<commit_message>
retrainig the model and adding css and js
</commit_message>
<xml_diff>
--- a/suivi_9_sites.xlsx
+++ b/suivi_9_sites.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="55">
   <si>
     <t>Code</t>
   </si>
@@ -173,10 +173,13 @@
     <t>CVC</t>
   </si>
   <si>
+    <t>Multi-usage</t>
+  </si>
+  <si>
+    <t>Investigation en cours</t>
+  </si>
+  <si>
     <t>Eclairage</t>
-  </si>
-  <si>
-    <t>Investigation en cours</t>
   </si>
 </sst>
 </file>
@@ -1304,7 +1307,7 @@
         <v>22</v>
       </c>
       <c r="P6" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="7" spans="1:16">
@@ -1354,7 +1357,7 @@
         <v>22</v>
       </c>
       <c r="P7" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
     </row>
     <row r="8" spans="1:16">
@@ -1504,7 +1507,7 @@
         <v>37</v>
       </c>
       <c r="P10" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="11" spans="1:16">
@@ -1554,7 +1557,7 @@
         <v>37</v>
       </c>
       <c r="P11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="12" spans="1:16">
@@ -1704,7 +1707,7 @@
         <v>30</v>
       </c>
       <c r="P14" t="s">
-        <v>31</v>
+        <v>54</v>
       </c>
     </row>
     <row r="15" spans="1:16">

</xml_diff>

<commit_message>
model of machine learning changed
</commit_message>
<xml_diff>
--- a/suivi_9_sites.xlsx
+++ b/suivi_9_sites.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="54">
   <si>
     <t>Code</t>
   </si>
@@ -110,6 +110,9 @@
     <t>70%</t>
   </si>
   <si>
+    <t>CVC</t>
+  </si>
+  <si>
     <t>Changement de comportement</t>
   </si>
   <si>
@@ -170,16 +173,10 @@
     <t>Nuit</t>
   </si>
   <si>
-    <t>CVC</t>
-  </si>
-  <si>
-    <t>Multi-usage</t>
+    <t>Eclairage</t>
   </si>
   <si>
     <t>Investigation en cours</t>
-  </si>
-  <si>
-    <t>Eclairage</t>
   </si>
 </sst>
 </file>
@@ -694,7 +691,7 @@
         <v>29</v>
       </c>
       <c r="P3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:16">
@@ -794,7 +791,7 @@
         <v>30</v>
       </c>
       <c r="P5" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:16">
@@ -844,7 +841,7 @@
         <v>30</v>
       </c>
       <c r="P6" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:16">
@@ -894,7 +891,7 @@
         <v>30</v>
       </c>
       <c r="P7" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:16">
@@ -944,7 +941,7 @@
         <v>30</v>
       </c>
       <c r="P8" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:16">
@@ -994,7 +991,7 @@
         <v>22</v>
       </c>
       <c r="P9" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -1062,7 +1059,7 @@
     </row>
     <row r="2" spans="1:16">
       <c r="A2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B2" t="s">
         <v>20</v>
@@ -1098,16 +1095,16 @@
         <v>2352</v>
       </c>
       <c r="M2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="N2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="O2" t="s">
         <v>22</v>
       </c>
       <c r="P2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:16">
@@ -1148,16 +1145,16 @@
         <v>3773</v>
       </c>
       <c r="M3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="N3" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="O3" t="s">
         <v>22</v>
       </c>
       <c r="P3" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:16">
@@ -1198,16 +1195,16 @@
         <v>1064</v>
       </c>
       <c r="M4" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="N4" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="O4" t="s">
         <v>29</v>
       </c>
       <c r="P4" t="s">
-        <v>51</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:16">
@@ -1248,21 +1245,21 @@
         <v>735</v>
       </c>
       <c r="M5" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="N5" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="O5" t="s">
         <v>29</v>
       </c>
       <c r="P5" t="s">
-        <v>52</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:16">
       <c r="A6" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B6" t="s">
         <v>20</v>
@@ -1298,21 +1295,21 @@
         <v>500</v>
       </c>
       <c r="M6" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="N6" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="O6" t="s">
         <v>22</v>
       </c>
       <c r="P6" t="s">
-        <v>53</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:16">
       <c r="A7" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B7" t="s">
         <v>20</v>
@@ -1348,16 +1345,16 @@
         <v>770</v>
       </c>
       <c r="M7" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="N7" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="O7" t="s">
         <v>22</v>
       </c>
       <c r="P7" t="s">
-        <v>54</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:16">
@@ -1398,21 +1395,21 @@
         <v>1505</v>
       </c>
       <c r="M8" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="N8" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="O8" t="s">
         <v>22</v>
       </c>
       <c r="P8" t="s">
-        <v>51</v>
+        <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:16">
       <c r="A9" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B9" t="s">
         <v>20</v>
@@ -1448,21 +1445,21 @@
         <v>1776</v>
       </c>
       <c r="M9" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="N9" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="O9" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="P9" t="s">
-        <v>53</v>
+        <v>31</v>
       </c>
     </row>
     <row r="10" spans="1:16">
       <c r="A10" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B10" t="s">
         <v>20</v>
@@ -1498,21 +1495,21 @@
         <v>198</v>
       </c>
       <c r="M10" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="N10" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="O10" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="P10" t="s">
-        <v>53</v>
+        <v>32</v>
       </c>
     </row>
     <row r="11" spans="1:16">
       <c r="A11" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B11" t="s">
         <v>20</v>
@@ -1548,16 +1545,16 @@
         <v>1494</v>
       </c>
       <c r="M11" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="N11" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="O11" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="P11" t="s">
-        <v>53</v>
+        <v>31</v>
       </c>
     </row>
     <row r="12" spans="1:16">
@@ -1598,21 +1595,21 @@
         <v>2730</v>
       </c>
       <c r="M12" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="N12" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="O12" t="s">
         <v>22</v>
       </c>
       <c r="P12" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="13" spans="1:16">
       <c r="A13" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B13" t="s">
         <v>20</v>
@@ -1648,21 +1645,21 @@
         <v>2460</v>
       </c>
       <c r="M13" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="N13" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="O13" t="s">
         <v>30</v>
       </c>
       <c r="P13" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="14" spans="1:16">
       <c r="A14" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B14" t="s">
         <v>20</v>
@@ -1698,21 +1695,21 @@
         <v>381</v>
       </c>
       <c r="M14" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="N14" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="O14" t="s">
         <v>30</v>
       </c>
       <c r="P14" t="s">
-        <v>54</v>
+        <v>32</v>
       </c>
     </row>
     <row r="15" spans="1:16">
       <c r="A15" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B15" t="s">
         <v>20</v>
@@ -1748,21 +1745,21 @@
         <v>101</v>
       </c>
       <c r="M15" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="N15" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="O15" t="s">
         <v>30</v>
       </c>
       <c r="P15" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="16" spans="1:16">
       <c r="A16" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B16" t="s">
         <v>20</v>
@@ -1798,16 +1795,16 @@
         <v>546</v>
       </c>
       <c r="M16" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="N16" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="O16" t="s">
         <v>30</v>
       </c>
       <c r="P16" t="s">
-        <v>53</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>